<commit_message>
added Matrix as csv., added Matrix to Latex file.
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
   <si>
     <t>Kosten</t>
   </si>
@@ -122,42 +122,18 @@
     <t>nein</t>
   </si>
   <si>
-    <t>Kinn, keine einschränkung</t>
-  </si>
-  <si>
     <t>vier bis fünf</t>
   </si>
   <si>
     <t>mittel</t>
   </si>
   <si>
-    <t>minimal</t>
-  </si>
-  <si>
-    <t>eigenständige Kontrolle über jeweilige Geste</t>
-  </si>
-  <si>
-    <t>unterschiedliche ausführung, faustgroß, größer</t>
-  </si>
-  <si>
-    <t>intuitive bewegung mit dem Kinn</t>
-  </si>
-  <si>
-    <t>Kontrollierte Kinnbeweugnen</t>
-  </si>
-  <si>
     <t>ja, nein bei opitscher Kopfsteuerung</t>
   </si>
   <si>
     <t>keine Einschränkung, ja bei optischer Kopfstuerung</t>
   </si>
   <si>
-    <t>minimal joystick, opitsche kopfstuerung schon schwer oder auch nur über kamera iphone dann leicht</t>
-  </si>
-  <si>
-    <t>teuer</t>
-  </si>
-  <si>
     <t>beschränkt</t>
   </si>
   <si>
@@ -167,33 +143,9 @@
     <t>ja, aufwendig</t>
   </si>
   <si>
-    <t>wartung ja</t>
-  </si>
-  <si>
-    <t>warutng nein, reinigung ja</t>
-  </si>
-  <si>
-    <t>laborsetting bzw. raum wo alles aufgebaut ist</t>
-  </si>
-  <si>
-    <t>elektroden sind nd schwer</t>
-  </si>
-  <si>
-    <t>kontrolle über muskelanspannungne</t>
-  </si>
-  <si>
-    <t>elektorden nicht groß, pads</t>
-  </si>
-  <si>
     <t>trial and error, gewöhungsbedürftig</t>
   </si>
   <si>
-    <t>teils, myo armband</t>
-  </si>
-  <si>
-    <t>warung ja</t>
-  </si>
-  <si>
     <t>ja bei invasiv und teilweise invasiv</t>
   </si>
   <si>
@@ -206,18 +158,12 @@
     <t>keine Einschränkungen</t>
   </si>
   <si>
-    <t>sehr klein</t>
-  </si>
-  <si>
     <t>messbare Gehirnsignale über 3.5 Hz</t>
   </si>
   <si>
     <t>je nach Anwendungsfall, für Desktopsteuerung fast keine (gibt bereits gratis Apps)</t>
   </si>
   <si>
-    <t>Mail antwort, eye tracking system plus mitgelieferte sdk oder eigene software schreiben</t>
-  </si>
-  <si>
     <t>ja wenn sich die Stimme verändert (zB. Stimmbruch) neu Kalibrieren</t>
   </si>
   <si>
@@ -249,6 +195,84 @@
   </si>
   <si>
     <t>verstaubte Brillengläser, zwei unterschiedliche Profile wenn einmal mit Kontaktlinsen und einmal mit Brille, Gläser sollen durchsichtig sein</t>
+  </si>
+  <si>
+    <t>Mail antwort, eye tracking system plus mitgelieferte sdk oder eigene software schreiben; Glasses 15.000$</t>
+  </si>
+  <si>
+    <t>550$ Quadstick, 350$ Chin Control, 2000€ Integra Mouse, Joystick low Budget</t>
+  </si>
+  <si>
+    <t>keine Einschränkung, bei optischer Methode ähnl Augensteuerung</t>
+  </si>
+  <si>
+    <t>etwas, interaktion funktioniert über Druck</t>
+  </si>
+  <si>
+    <t>nein, ja bei optischer Variante</t>
+  </si>
+  <si>
+    <t>warutng nein, reinigung ja z.B. bei Mundsteuerung</t>
+  </si>
+  <si>
+    <t>minimal joystick, opitsche kopfstuerung je nachdem wo die Kamera positioniert ist</t>
+  </si>
+  <si>
+    <t>minimal, Bewungsrichtungen des Joysticks sind intuitv</t>
+  </si>
+  <si>
+    <t>eigenständige Kontrolle über das jeweilige Körperteil</t>
+  </si>
+  <si>
+    <t>Mundsteuerungen bzw. gewöhnliche Joysticks ungefähr Faustgroß, andere Systeme etwas größer</t>
+  </si>
+  <si>
+    <t>intuitive bewegung mit dem Kinn, Füßen und Kopf, kurze Eingewöhnungsphase bei Mundsteuerung (saugen, blasen)</t>
+  </si>
+  <si>
+    <t>Kontrollierte Bewegungen der ausgewählten Körperteile</t>
+  </si>
+  <si>
+    <t>System muss auf Benutzer genau angepasst werden, wenn die Bewegungen sehr rucksartig sind</t>
+  </si>
+  <si>
+    <t>200$ Myo Band</t>
+  </si>
+  <si>
+    <t>ja vor jeder Benützung</t>
+  </si>
+  <si>
+    <t>Myo Armband ja, ansonten nein</t>
+  </si>
+  <si>
+    <t>Laborsetting , keine Einschränkung bei Myo Armband</t>
+  </si>
+  <si>
+    <t>Kontrolliertes Anspannen und Entspannen der Muskeln</t>
+  </si>
+  <si>
+    <t>Je nach Produkt, Elektroden an sich nicht groß, Myo-Armband: 11,9 x 7,4 x 10,4 cm</t>
+  </si>
+  <si>
+    <t>Myo Armband 254g</t>
+  </si>
+  <si>
+    <t>Kontrolle über muskelanspannungne</t>
+  </si>
+  <si>
+    <t>Richtige Positionierung der Elektroden, damit genug Muskelaktivität gemessen werden kann</t>
+  </si>
+  <si>
+    <t>keine Produkte am Markt bisher</t>
+  </si>
+  <si>
+    <t>Elektroden an sich minimal</t>
+  </si>
+  <si>
+    <t>Größer der Elektroden - sehr klein</t>
+  </si>
+  <si>
+    <t>Noch keine Produkte auf dem Markt bzw. 100% sicher erprobtes System, Risiko bei der Operation zur Elektrodeneinsetzung</t>
   </si>
 </sst>
 </file>
@@ -312,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -342,6 +366,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,16 +696,17 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -686,26 +724,28 @@
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -716,19 +756,19 @@
         <v>25</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>50</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -736,16 +776,16 @@
         <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -758,14 +798,14 @@
       <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>46</v>
+      <c r="D5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -773,19 +813,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>55</v>
+      <c r="D6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -799,16 +839,16 @@
         <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -816,36 +856,36 @@
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
+        <v>53</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -853,13 +893,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -870,19 +916,19 @@
         <v>29</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -892,37 +938,37 @@
       <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="D12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -930,16 +976,16 @@
         <v>20</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -952,14 +998,14 @@
       <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>61</v>
+      <c r="D15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -970,11 +1016,17 @@
         <v>27</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>